<commit_message>
Added block about the most important markers in explanation
</commit_message>
<xml_diff>
--- a/models/Immunomarkers/Immunomarkers.xlsx
+++ b/models/Immunomarkers/Immunomarkers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\EpImAge\models\Immunomarkers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9398167-73E4-4167-AAB6-18AF6ABA5C25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{324F08F7-4203-476E-B315-8329DF074E46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="86">
   <si>
     <t>feature</t>
   </si>
@@ -208,6 +208,85 @@
   </si>
   <si>
     <t>130 T</t>
+  </si>
+  <si>
+    <t>Text</t>
+  </si>
+  <si>
+    <t>#### CXCL9 
+C-X-C motif chemokine ligand 9, also known as monokine induced by gamma interferon (MIG) is one of the most age-associated chemokines [[1](https://doi.org/10.1038/s43587-021-00082-y), [2](https://doi.org/10.3389/fimmu.2023.1177611)]. It is also involved in cardiac aging and vascular function [[1](https://doi.org/10.1038/s43587-021-00082-y)], regulation of chronic inflammation and inflammaging [[1](https://doi.org/10.1038/s43587-021-00082-y), [2](https://doi.org/10.3389/fimmu.2023.1177611), [3](https://doi.org/10.1007/s00198-024-07160-y)]. Levels of this biomarker may be elevated in primary Sjögren's syndrome [[4](https://doi.org/10.1186/s13075-023-03229-x)], Chagas disease [[5](https://doi.org/10.1186%2Fs40249-020-00663-w)], chronic renal failure [[7](https://doi.org/10.1007/s11357-022-00540-4)], during progression of sarcoidosis [[6](https://doi.org/10.1016%2Fj.rmed.2019.105822)], and also be associated with age-related changes in muscle strength [[3](https://doi.org/10.1007/s00198-024-07160-y)] and frailty [[8](https://doi.org/10.1159/000535109)] in the elderly. Its concentration also varies in different types of cancer and may be a marker of the effectiveness of cancer treatment [[9](https://doi.org/10.1016%2Fj.ctrv.2017.11.007)].</t>
+  </si>
+  <si>
+    <t>#### CCL2
+C-C motif chemokine ligand 2, also known as monocyte chemotactic protein 1 (MCP-1) is a proinflammatory chemokine [[1](https://doi.org/10.1089%2Fjir.2008.0027)] associated with a wide range of diseases: rheumatoid arthritis [[2](https://europepmc.org/article/med/20017457)], diabetes [[3](https://doi.org/10.1016/j.cyto.2012.06.018)], congestive heart failure [[4](https://doi.org/10.1161/01.CIR.97.12.1136)], Schnitzler syndrome [[5](https://doi.org/10.1111/bjd.17334)], chronic traumatic encephalopathy [[6](https://doi.org/10.1186/s12974-020-02036-4)], dyslipidemia in cardiovascular and renal diseases [[7](https://doi.org/10.1016/j.cyto.2019.154858)] and in many other pathologies [[8](https://doi.org/10.3389/fimmu.2019.02759)]. Abnormal CCL2 levels in pregnancy may indicate risks of spontaneous abortion, preeclampsia and preterm labor [[9](https://doi.org/10.3389%2Ffimmu.2022.1053457)].</t>
+  </si>
+  <si>
+    <t>#### IL-6
+Interleukin-6 is a multifunctional cytokine that plays an important role in the protection of the human body and in affecting chronic inflammation and autoimmunity [[1](https://doi.org/10.1002%2Fpro.5560060501), [2](https://doi.org/10.1101%2Fcshperspect.a016295)]. Its levels increase with age [[3](https://doi.org/10.1186%2Fs12979-016-0076-x)] and may be associated with the risk of a wide range of diseases, including cardiovascular diseases [[4](https://doi.org/10.1186/s12916-022-02446-6)], autoimmune diseases [[5](https://doi.org/10.3389/fimmu.2023.1255533)], cancer [[6](https://doi.org/10.1093%2Fgerona%2F61.6.575)], type 2 diabetes [[7](https://doi.org/10.1001/jama.286.3.327)], rheumatoid arthritis [[8](https://doi.org/10.1002/art.1780310614)], and mortality risk, particularly from cardiovascular diseases [[9](https://doi.org/10.1016/S0002-9343(99)00066-2)].</t>
+  </si>
+  <si>
+    <t>#### CCL11</t>
+  </si>
+  <si>
+    <t>#### IL27</t>
+  </si>
+  <si>
+    <t>#### IL5</t>
+  </si>
+  <si>
+    <t>#### IL1B</t>
+  </si>
+  <si>
+    <t>#### GCSF</t>
+  </si>
+  <si>
+    <t>#### CXCL10</t>
+  </si>
+  <si>
+    <t>#### VEGFA</t>
+  </si>
+  <si>
+    <t>#### TNF</t>
+  </si>
+  <si>
+    <t>#### PDGFB</t>
+  </si>
+  <si>
+    <t>#### IL8</t>
+  </si>
+  <si>
+    <t>#### PDGFA</t>
+  </si>
+  <si>
+    <t>#### IL12Bp40</t>
+  </si>
+  <si>
+    <t>#### IL15</t>
+  </si>
+  <si>
+    <t>#### CXCL1</t>
+  </si>
+  <si>
+    <t>#### CCL4</t>
+  </si>
+  <si>
+    <t>#### IFNA2</t>
+  </si>
+  <si>
+    <t>#### IL13</t>
+  </si>
+  <si>
+    <t>#### FLT3L</t>
+  </si>
+  <si>
+    <t>#### CD40LG</t>
+  </si>
+  <si>
+    <t>#### CCL22</t>
+  </si>
+  <si>
+    <t>#### CSF-1
+Colony Stimulating Factor-1 is one of the best known proinflammatory cytokines responsible for a variety of inflammatory diseases [[1](https://doi.org/10.1016/j.biopha.2018.04.046)]. Its levels depend on age [[2](https://doi.org/10.1038/s41598-017-07698-4), [3](https://doi.org/10.3389/fimmu.2023.1177611)] and can be associated with bad habits, including smoking [[4](https://doi.org/10.1038/s41598-017-07698-4)], as well as with various diseases such as periodontitis [[4](https://doi.org/10.1038/s41598-017-07698-4)], chronic kidney disease [[5](https://doi.org/10.1007%2Fs11357-022-00540-4)], atherosclerosis and cancer [[6](https://doi.org/10.1016/j.coi.2005.11.006)].</t>
   </si>
 </sst>
 </file>
@@ -271,7 +350,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -282,6 +361,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -563,10 +645,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S25"/>
+  <dimension ref="A1:T25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="Y15" sqref="Y15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="6" ySplit="27" topLeftCell="M31" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="G1" sqref="G1"/>
+      <selection pane="bottomLeft" activeCell="A28" sqref="A28"/>
+      <selection pane="bottomRight" activeCell="T12" sqref="T12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -590,10 +675,11 @@
     <col min="17" max="17" width="20.54296875" style="3" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="6.90625" style="3" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="6.6328125" style="3" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="8.7265625" style="3"/>
+    <col min="20" max="20" width="134.81640625" style="3" customWidth="1"/>
+    <col min="21" max="16384" width="8.7265625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -651,8 +737,11 @@
       <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T1" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>19</v>
       </c>
@@ -710,8 +799,11 @@
       <c r="S2" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T2" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>22</v>
       </c>
@@ -769,8 +861,11 @@
       <c r="S3" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T3" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>25</v>
       </c>
@@ -828,8 +923,11 @@
       <c r="S4" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T4" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>27</v>
       </c>
@@ -887,8 +985,11 @@
       <c r="S5" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T5" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>29</v>
       </c>
@@ -946,8 +1047,11 @@
       <c r="S6" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T6" s="5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>31</v>
       </c>
@@ -1005,8 +1109,11 @@
       <c r="S7" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T7" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>33</v>
       </c>
@@ -1064,8 +1171,11 @@
       <c r="S8" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T8" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" ht="20.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>35</v>
       </c>
@@ -1123,8 +1233,11 @@
       <c r="S9" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T9" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>36</v>
       </c>
@@ -1182,8 +1295,11 @@
       <c r="S10" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T10" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>37</v>
       </c>
@@ -1241,8 +1357,11 @@
       <c r="S11" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T11" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>39</v>
       </c>
@@ -1300,8 +1419,11 @@
       <c r="S12" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T12" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>41</v>
       </c>
@@ -1359,8 +1481,11 @@
       <c r="S13" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T13" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>42</v>
       </c>
@@ -1418,8 +1543,11 @@
       <c r="S14" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T14" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
         <v>44</v>
       </c>
@@ -1477,8 +1605,11 @@
       <c r="S15" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T15" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
         <v>45</v>
       </c>
@@ -1536,8 +1667,11 @@
       <c r="S16" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T16" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
         <v>46</v>
       </c>
@@ -1595,8 +1729,11 @@
       <c r="S17" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T17" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
         <v>47</v>
       </c>
@@ -1654,8 +1791,11 @@
       <c r="S18" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T18" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
         <v>49</v>
       </c>
@@ -1713,8 +1853,11 @@
       <c r="S19" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T19" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
         <v>51</v>
       </c>
@@ -1772,8 +1915,11 @@
       <c r="S20" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T20" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
         <v>53</v>
       </c>
@@ -1831,8 +1977,11 @@
       <c r="S21" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T21" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
         <v>54</v>
       </c>
@@ -1890,8 +2039,11 @@
       <c r="S22" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T22" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
         <v>56</v>
       </c>
@@ -1949,8 +2101,11 @@
       <c r="S23" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T23" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
         <v>58</v>
       </c>
@@ -2008,8 +2163,11 @@
       <c r="S24" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T24" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A25" s="4" t="s">
         <v>59</v>
       </c>
@@ -2066,6 +2224,9 @@
       </c>
       <c r="S25" s="3">
         <v>5</v>
+      </c>
+      <c r="T25" s="4" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Immunomarkers info added, typos fixed
</commit_message>
<xml_diff>
--- a/models/Immunomarkers/Immunomarkers.xlsx
+++ b/models/Immunomarkers/Immunomarkers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\EpImAge\models\Immunomarkers\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EpImAge\models\Immunomarkers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{324F08F7-4203-476E-B315-8329DF074E46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF34D271-A1AC-4A19-9E0E-AF5D95CCC8EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="735" yWindow="1980" windowWidth="20520" windowHeight="18225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -213,79 +213,99 @@
     <t>Text</t>
   </si>
   <si>
-    <t>#### CXCL9 
-C-X-C motif chemokine ligand 9, also known as monokine induced by gamma interferon (MIG) is one of the most age-associated chemokines [[1](https://doi.org/10.1038/s43587-021-00082-y), [2](https://doi.org/10.3389/fimmu.2023.1177611)]. It is also involved in cardiac aging and vascular function [[1](https://doi.org/10.1038/s43587-021-00082-y)], regulation of chronic inflammation and inflammaging [[1](https://doi.org/10.1038/s43587-021-00082-y), [2](https://doi.org/10.3389/fimmu.2023.1177611), [3](https://doi.org/10.1007/s00198-024-07160-y)]. Levels of this biomarker may be elevated in primary Sjögren's syndrome [[4](https://doi.org/10.1186/s13075-023-03229-x)], Chagas disease [[5](https://doi.org/10.1186%2Fs40249-020-00663-w)], chronic renal failure [[7](https://doi.org/10.1007/s11357-022-00540-4)], during progression of sarcoidosis [[6](https://doi.org/10.1016%2Fj.rmed.2019.105822)], and also be associated with age-related changes in muscle strength [[3](https://doi.org/10.1007/s00198-024-07160-y)] and frailty [[8](https://doi.org/10.1159/000535109)] in the elderly. Its concentration also varies in different types of cancer and may be a marker of the effectiveness of cancer treatment [[9](https://doi.org/10.1016%2Fj.ctrv.2017.11.007)].</t>
-  </si>
-  <si>
     <t>#### CCL2
 C-C motif chemokine ligand 2, also known as monocyte chemotactic protein 1 (MCP-1) is a proinflammatory chemokine [[1](https://doi.org/10.1089%2Fjir.2008.0027)] associated with a wide range of diseases: rheumatoid arthritis [[2](https://europepmc.org/article/med/20017457)], diabetes [[3](https://doi.org/10.1016/j.cyto.2012.06.018)], congestive heart failure [[4](https://doi.org/10.1161/01.CIR.97.12.1136)], Schnitzler syndrome [[5](https://doi.org/10.1111/bjd.17334)], chronic traumatic encephalopathy [[6](https://doi.org/10.1186/s12974-020-02036-4)], dyslipidemia in cardiovascular and renal diseases [[7](https://doi.org/10.1016/j.cyto.2019.154858)] and in many other pathologies [[8](https://doi.org/10.3389/fimmu.2019.02759)]. Abnormal CCL2 levels in pregnancy may indicate risks of spontaneous abortion, preeclampsia and preterm labor [[9](https://doi.org/10.3389%2Ffimmu.2022.1053457)].</t>
   </si>
   <si>
-    <t>#### IL-6
+    <t>#### CXCL9 
+C-X-C motif chemokine ligand 9, also known as monokine induced by gamma interferon (MIG) is one of the most age-associated chemokines [[1](https://doi.org/10.1038/s43587-021-00082-y), [2](https://doi.org/10.3389/fimmu.2023.1177611)]. It is also involved in cardiac aging and vascular function [[1](https://doi.org/10.1038/s43587-021-00082-y)], regulation of chronic inflammation and inflammaging [[1](https://doi.org/10.1038/s43587-021-00082-y), [2](https://doi.org/10.3389/fimmu.2023.1177611), [3](https://doi.org/10.1007/s00198-024-07160-y)]. Levels of this biomarker may be elevated in primary Sjögren's syndrome [[4](https://doi.org/10.1186/s13075-023-03229-x)], Chagas disease [[5](https://doi.org/10.1186%2Fs40249-020-00663-w)], chronic renal failure [[6](https://doi.org/10.1007/s11357-022-00540-4)], during progression of sarcoidosis [[7](https://doi.org/10.1016%2Fj.rmed.2019.105822)], and also be associated with age-related changes in muscle strength [[3](https://doi.org/10.1007/s00198-024-07160-y)] and frailty [[8](https://doi.org/10.1159/000535109)] in the elderly. Its concentration also varies in different types of cancer and may be a marker of the effectiveness of cancer treatment [[9](https://doi.org/10.1016%2Fj.ctrv.2017.11.007)].</t>
+  </si>
+  <si>
+    <t>#### IL27
+Interleukin-27 is a multifunctional cytokine that combines pro- and anti-inflammatory properties [[1](https://doi.org/10.1038/nri1648)] and can both promote and inhibit the development of inflammatory diseases, cancer, and viral infections [[2](https://doi.org/10.3389/fimmu.2023.1191228), [3](https://doi.org/10.3389/fimmu.2021.678515)]. IL27 expression is abnormal in various inflammatory autoimmune diseases (systemic lupus erythematosus, rheumatoid arthritis, Sjögren's syndrome, Behçet's disease, inflammatory bowel disease, multiple sclerosis, systemic sclerosis, and type 1 diabetes) [[4](https://doi.org/10.3389/fimmu.2024.1366377), [5](https://doi.org/10.1080/08830185.2020.1840565)]. IL27 has neuroprotective activity in the retina and brain [[6](https://doi.org/10.4103/1673-5374.336134)]. In COVID-19, its levels are positively correlated with advanced age, prolonged hospitalization, and severe disease [[7](https://doi.org/10.1038/s41419-020-03151-z)].</t>
+  </si>
+  <si>
+    <t>#### IL5
+Interleukin-5 is a key cytokine that mediates eosinophil activation and is involved in the development of many eosinophil-related diseases such as asthma, allergic rhinitis, and eosinophilic esophagitis [[1](https://doi.org/10.1016/B978-0-7234-3691-1.00105-7), [2](https://doi.org/10.1016/j.immuni.2019.03.022), [3](https://doi.org/10.1093/intimm/dxp102)]. Suppression of IL5 action by humanized anti-IL-5 monoclonal antibody can be used to treat asthma and other respiratory diseases [[4](https://doi.org/10.2183/pjab.87.463), [5](https://doi.org/10.3389/fphys.2019.01514), [6](https://doi.org/10.1111/all.16303)]. Decreased IL5 levels may be associated with coronary heart disease, as well as with the risk of angina pectoris and acute myocardial infarction [[7](https://doi.org/10.1016/j.rec.2019.07.005)].</t>
+  </si>
+  <si>
+    <t>#### IL1B
+Interleukin-1 Beta is a cytokine that plays an important role in enhancing immune response, a defense mechanism against pathogens and short-term inflammation [[1](https://doi.org/10.2119/molmed.2014.00232), [2](https://doi.org/10.1016/j.obmed.2021.100375), [3](https://doi.org/10.1038/cmi.2016.25)]. IL1B levels are responsible for the progression of obesity and impaired insulin signaling [[4](https://doi.org/10.4161/21623945.2014.979661)] and are associated with metabolic syndrome, invasiveness and progression of cancer [[5](https://doi.org/10.1186/s41232-019-0101-5)]. Elevated IL1B concentration is associated with worsening reproductive dysfunction in women with polycystic ovary syndrome [[6](https://doi.org/10.1016/s1995-7645(13)60030-9)], as well as with the intensity of inflammation in inflammatory bowel disease [[7](https://doi.org/10.3389/fmed.2024.1307394)]. IL1B plays a key role in intervertebral disc degeneration [[8](https://doi.org/10.1016/j.jcm.2017.09.003)], and its elevated levels are associated with autoinflammatory diseases [[9](https://doi.org/10.1182/blood-2010-07-273417)].</t>
+  </si>
+  <si>
+    <t>#### VEGFA
+Vascular Endothelial Growth Factor A is a cytokine that actively participates in inflammatory processes and is involved in angiogenesis, lymphangiogenesis, and hematopoiesis [[1](https://doi.org/10.1016/j.cyto.2012.10.024)]. Elevated levels of circulating VEGF have been observed in ischemic heart disease, diabetes, reproductive and inflammatory diseases [[1](https://doi.org/10.1016/j.cyto.2012.10.024), [2](https://doi.org/10.1016/j.thromres.2008.06.014)]. Increased VEGF expression contributes to the pathogenesis of inflammatory lung diseases [[3](https://doi.org/10.1155/2015/387842)], chronic inflammation in age-related macular degeneration [[4](https://doi.org/10.1002/jcp.22708)], as well as the development of cataracts, neovascular and non-exudative ocular pathologies [[5](https://doi.org/10.15252/emmm.201505613)]. Inhibition of VEGFA in the umbilical cord has been associated with negative pregnancy outcomes [[6](https://doi.org/10.1016/j.placenta.2019.09.002)].</t>
+  </si>
+  <si>
+    <t>#### TNF
+Tumor Necrosis Factor is a pro-inflammatory cytokine that exerts various effects in response to acute inflammation [[1](https://doi.org/10.1016/bs.acc.2022.06.002), [2](https://doi.org/10.2174/1389450120666190821161259)]. In the healthy brain, baseline TNF-α release modulates plasticity for memory and learning processes [[3](https://doi.org/10.1038/nature04671)]; in neuroinflammation, increased TNF-α expression is associated with cytotoxicity and memory impairment [[4](https://doi.org/10.1007/s11481-011-9287-2)]. TNF has been implicated in a wide range of diseases such as cancer, arthritis, diabetes and other inflammatory diseases [[5](https://doi.org/10.1016/j.preteyeres.2005.09.001), [6](https://doi.org/10.2174/1568010023344571)]. Abnormal levels of TNF have been observed in rheumatoid arthritis, inflammatory bowel disease, psoriatic arthritis, psoriasis and uveitis [[7](https://doi.org/10.3390/ijms22052719)]. TNF is involved in the pathogenesis of atherosclerosis, type 2 diabetes mellitus, and Alzheimer's disease in the elderly. Age-related increases in systemic TNF levels are associated with frailty and mortality risks [[8](https://doi.org/10.1016/s0889-8561(02)00056-5)].</t>
+  </si>
+  <si>
+    <t>#### PDGFB
+Platelet Derived Growth Factor B is a cytokine that plays an important role in the development and differentiation of the vascular wall [[1](https://doi.org/10.1016/j.jocn.2009.02.009)]. Its elevated levels are observed in systemic lupus erythematosus [[2](https://doi.org/10.1186/s13075-017-1238-8)] and can be associated with an increased risk of acute myocardial infarction [[3](https://doi.org/10.18632/aging.205413)]. Increased PDGFB levels were observed in patients with ankylosing spondylitis and were associated with disease progression [[4](https://doi.org/10.1002/jbmr.4751)].</t>
+  </si>
+  <si>
+    <t>#### PDGFA
+Platelet Derived Growth Factor A is a cytokine that plays an important role in bone metabolism [[1](https://doi.org/10.1006/cyto.2000.0707)]. Decreased serum and pancreatic PDGFA levels contribute to decreased pancreatic function in aging [[2](https://doi.org/10.1016/j.bbrc.2019.12.057)]. PDGFA may be associated with different types of cancer [[3](https://doi.org/10.1006/excr.1993.1195), [4](https://doi.org/10.1016/0165-4608(94)90195-3)].</t>
+  </si>
+  <si>
+    <t>#### IL12Bp40
+Interleukin-12 Beta subunit p40 is a cytokine that affects susceptibility to mycobacteria [[1](https://doi.org/10.1016/S0891-5520(03)00051-5)], acts as a chemoattractant for macrophages and promotes migration of bacteria-stimulated dendritic cells [[2](https://doi.org/10.1016/j.it.2006.11.002)]. The observed levels of IL12p40 increase with age [[3](https://doi.org/10.1006/cyto.1999.0537)]. IL12p40 is important for pathologies associated with psoriasis, inflammatory bowel disease and tumor growth [[4](https://doi.org/10.1016/j.cytogfr.2014.07.017), [5](https://doi.org/10.1111/exd.14566)], and IL12p40 deficiency abrogates IL17 production and prevents autoimmune response [[6](https://doi.org/10.1016/j.intimp.2006.09.024)]. Increased expression of IL12B has been observed in the central nervous system of patients with multiple sclerosis [[7](https://doi.org/10.1016/j.cyto.2017.10.024)], as well as in patients with hepatitis B [[8](https://doi.org/10.1016/j.meegid.2020.104663)].</t>
+  </si>
+  <si>
+    <t>#### IFNA2
+Interferon Alpha-2 is a pro-inflammatory cytokine secreted by virus-infected cells and acts to suppress viral infection [[1](https://doi.org/10.1016/j.gene.2015.04.087)]. Elevated IFNA2 levels are associated with systemic lupus erythematosus [[2](https://doi.org/10.1136/annrheumdis-2024-eular.4199), [3](https://doi.org/10.1177/0961203312468964)], rheumatoid arthritis [[4](https://doi.org/10.1038/s41598-024-72564-z)] and Sjögren's syndrome [[5](https://doi.org/10.1093/rheumatology/keab688)], and are also increased in patients with COVID-19 [[6](https://doi.org/10.3389/fimmu.2023.1250214)].</t>
+  </si>
+  <si>
+    <t>#### IL13
+Interleukin-13 is a cytokine with pro-inflammatory and anti-inflammatory properties, one of the central regulators of eosinophilic diseases [[1](https://doi.org/10.1016/j.anai.2012.06.014)], plays an important role in atopic disorders [[2](https://doi.org/10.1016/j.giec.2017.07.011), [3](https://doi.org/10.1111/all.13954)] and regulates many aspects of allergic inflammation [[3](https://doi.org/10.1111/all.13954), [4](https://doi.org/10.3389/fimmu.2018.00888)]. IL13 is involved in the pathogenesis of autoimmune diseases such as systemic lupus erythematosus, rheumatoid arthritis, systemic sclerosis, ulcerative colitis, type 1 diabetes, and Sjögren's syndrome [[5](https://doi.org/10.1016/j.cytogfr.2018.12.001)]. IL13 levels are elevated in age-related macular degeneration [[6](https://doi.org/10.18240/ijo.2017.04.06)], and decrease with age in joints [[7](https://doi.org/10.1016/j.ocarto.2020.100128)].</t>
+  </si>
+  <si>
+    <t>#### FLT3L
+Fms-related tyrosine kinase 3 ligand is a cytokine, an important regulator of hematopoiesis [[1](https://doi.org/10.3390/ijms18061115)]; its deficiency impairs monocyte development [[2](https://doi.org/10.1016/j.cell.2024.04.009)]. Elevated levels of FLT3L are observed in malaria and inflammatory bowel disease [[3](https://doi.org/10.1038/s41598-017-18283-0)], it is actively involved in acute myeloid leukemia [[4](https://doi.org/10.3390/ijms18061115), [5](https://doi.org/10.1016/j.autrev.2013.09.010)].</t>
+  </si>
+  <si>
+    <t>#### CCL11
+CC-motif chemokine ligand 11, also known as eosinophil chemotactic protein (Eotaxin-1) is a chemokine that acts as a chemoattractant for eosinophilic granulocytes [[1](https://doi.org/10.1073/pnas.95.11.6273)] and is involved in the development of numerous diseases, associated with eosinophils, such as atopic dermatitis, allergic rhinitis, sinusitis, asthma, ulcerative colitis [[2](https://doi.org/10.3389/fnagi.2017.00402), [3](https://doi.org/10.1007/s00405-012-1927-5), [4](https://doi.org/10.3389/fimmu.2023.1243537)], as well as in the response to parasitic infections [[5](https://doi.org/10.1111/tmi.12095)], vascular inflammation and atherosclerosis [[6](https://doi.org/10.1161/01.CIR.102.18.2185)]. Age- related increases in CCL11 are associated with cognitive impairment, elevated CCL11 levels have been observed in psychiatric disorders as well as increased risk of Alzheimer's disease and multiple sclerosis [[7](https://doi.org/10.3390/ph13090230), [8](https://doi.org/10.3389/fpsyt.2018.00241)].</t>
+  </si>
+  <si>
+    <t>#### GCSF
+Granulocyte Colony-Stimulating Factor, also known as colony-stimulating factor 3 (CSF3), is a cytokine that plays a key role in the regulation of neutrophil production [[1](https://doi.org/10.1016/j.molimm.2015.12.006)] and stimulates the proliferation and differentiation of stem cells into mature granulocytes [[2](https://doi.org/10.1016/B978-1-4377-2662-6.00018-3)]. It affects oocyte maturation and embryonic development [[3](https://doi.org/10.1016/B978-0-323-90805-4.00017-1)]. Elevated GCSF levels may lead to neutrophil abnormalities in severe COVID-19 [[4](https://doi.org/10.1002/JLB.3CE0121-002R)]. GCSF is elevated in age-related macular degeneration [[5](https://iovs.arvojournals.org/article.aspx?articleid=2790739)], has a contrasting effect in arthritis and inflammatory bowel diseases [[6](https://doi.org/10.1002/iub.361)].</t>
+  </si>
+  <si>
+    <t>#### CXCL10
+C-X-C motif chemokine ligand 10, also known as  interferon gamma-induced protein 10 (IP-10) is a chemokine actively involved in regulating immune responses [[1](https://doi.org/10.1016/j.autrev.2008.12.002)]. CXCL10 levels are increased in various autoimmune diseases such as rheumatoid arthritis, systemic lupus erythematosus, Sjögren's syndrome, systemic sclerosis, idiopathic inflammatory myopathy, and Chagas disease [[1](https://doi.org/10.1016/j.autrev.2008.12.002), [2](https://doi.org/10.1016/j.cyto.2021.155640), [3](https://doi.org/10.1186/s40249-020-00663-w)]. CXCL10 is involved in response to infections including rhinovirus [[4](https://doi.org/10.1164/rccm.200911-1673OC)], coxsackie virus, hepatitis B and C viruses [[5](https://doi.org/10.1002/jmv.10431)]. CXCL10 protects against severe acute respiratory syndrome caused by coronavirus [[6](https://doi.org/10.1016/j.cytogfr.2011.06.001), [7](https://doi.org/10.1186/s12979-024-00430-7)]. The observed levels of CXCL10 were higher in elderly compared to young adults and were negatively associated with working memory performance and higher in people with Alzheimer's disease [[8](https://doi.org/10.1016/j.neurobiolaging.2017.11.009)].</t>
+  </si>
+  <si>
+    <t>#### IL8
+IInterleukin-8, also known as C-X-C motif chemokine ligand 8 (CXCL8), is a proinflammatory chemokine that activates neutrophils [[1](https://pubmed.ncbi.nlm.nih.gov/8315568/)] and is clinically used as a biomarker of inflammation [[2](https://doi.org/10.1159/000514885)]. Spontaneous IL8 secretion is lower in the elderly than in the young [[3](https://doi.org/10.1016/0047-6374(94)90020-5)]; however, blood IL8 concentration increases with age [[4](https://doi.org/10.1186/s12979-019-0151-1)] and in response to pain, and may characterize age-related dysregulation of the immune system [[5](https://doi.org/10.1016/j.exger.2015.09.017)]. IL8 is involved in the establishment and maintenance of the inflammatory microenvironment of the damaged vascular wall in cadiovascular diseases [[6](https://doi.org/10.1093/cvr/cvp241)], and its increase is associated with disease severity and prognosis for COVID-19 patients [[7](https://doi.org/10.3389/fimmu.2020.602395), [8](https://doi.org/10.3390/v15020549)].</t>
+  </si>
+  <si>
+    <t>#### CXCL1
+C-X-C motif chemokine ligand 1, also known as Growth-Regulated Oncogene alpha (GROa) is a cytokine, a neutrophil chemoattractant that plays an important role in the activation of innate immunity [[1](https://doi.org/10.1016/j.brainresbull.2021.05.024)]. CXCL1 induces regeneration of dopaminergic nerves [[2](https://doi.org/10.1016/j.brainresbull.2019.05.020)] and is elevated in chronic obstructive pulmonary disease and in smokers [[3](https://doi.org/10.1016/j.tips.2006.08.001)]. Plasma CXCL1 levels were elevated in patients with high-functioning autism spectrum disorder [[4](https://doi.org/10.1371/journal.pone.0020470)]. CXCL1 is involved in diseases of the cardiovascular system (atherosclerosis, atrial fibrillation, chronic ischemic heart disease, hypertension, sepsis), respiratory system (asthma, chronic obstructive pulmonary disease, rhinosinusitis, COVID-19, influenza, tuberculosis), skin (wound healing, psoriasis, burns), musculoskeletal system (osteoporosis, rheumatoid arthritis) [[5](https://doi.org/10.3390/ijms24010205), [6](https://doi.org/10.3390/ijms23084205), [7](https://doi.org/10.1038/s41420-023-01524-9)].</t>
+  </si>
+  <si>
+    <t>#### CCL4
+C-C motif ligand 4, also known as Macrophage Inflammatory Protein 1 Beta (MIP-1b) is a proinflammatory chemokine that is released by activated cells in response to inflammation and regulates antitumor immunity [[1](https://doi.org/10.1016/j.semcancer.2022.06.010)]. Elevated levels of CCL4 are observed in systemic sclerosis, some infectious and bacterial diseases [[2](https://doi.org/10.1016/B978-0-08-102723-3.00252-3)]. CCL4 has been found to be associated with the pathogenesis of cardiovascular diseases, diabetes mellitus, autoimmune disorders, and HIV infection [[3](https://doi.org/10.1186/s12933-016-0439-9), [4](https://doi.org/10.1016/j.dci.2022.104525)]. CCL4 plays a key role in adipose tissue monocyte recruitment and demonstrate increased production in obesity [[5](https://doi.org/10.3390/ijms20184658)]. Circulating CCL4 increases with age [[6](https://doi.org/10.1007/s10456-024-09922-y)].</t>
+  </si>
+  <si>
+    <t>#### CD40LG
+CD40 ligand is a cytokine that plays an important role in humoral responses, vascular physiopathology [[1](https://doi.org/10.1016/j.imbio.2011.03.010)], adaptive immunity [[2](https://doi.org/10.3389/fcvm.2017.00040)], and activation in response to inflammation [[3](https://doi.org/10.4049/jimmunol.168.2.713)]. It is involved in the effects of rheumatoid arthritis on bone [[4](https://doi.org/10.1016/B978-0-12-415853-5.00038-8)], atherosclerosis and other cardiovascular pathologies [[1](https://doi.org/10.1016/j.imbio.2011.03.010), [5](https://doi.org/10.3390/ijms21228533)]. CD40LG (and the CD40-CD40LG axis) is active in systemic lupus erythematosus [[6](https://doi.org/10.1016/j.clim.2009.05.011)], inflammatory bowel disease [[7](https://doi.org/10.3389/fimmu.2015.00529)], and other autoimmune diseases [[8](https://doi.org/10.1016/j.addr.2018.12.005)], as well as in central nervous system pathologies including brain injury, Alzheimer's disease, Parkinson's disease, stroke, epilepsy, and multiple sclerosis [[9](https://doi.org/10.3390/ijms23084115)].</t>
+  </si>
+  <si>
+    <t>#### CCL22
+C-C motif ligand 22, also known as Macrophage-Derived Chemokine (MDC) is a chemokine involved in the transportation of cells to the focus of inflammation [[1](https://doi.org/10.1016/j.intimp.2020.106314)]. Decreased levels of CCL22 have been observed in patients with multiple sclerosis [[2](https://doi.org/10.1007/s10753-013-9775-z)], COVID-19 [[3](https://doi.org/10.3390/ijms241713083)]. Increased production of CCL22 is observed in parasitic infections [[4](https://doi.org/10.1016/j.cytogfr.2022.05.002)], psychotic disorders [[5](https://doi.org/10.1038/s41398-020-0776-z)].</t>
+  </si>
+  <si>
+    <t>#### IL6
 Interleukin-6 is a multifunctional cytokine that plays an important role in the protection of the human body and in affecting chronic inflammation and autoimmunity [[1](https://doi.org/10.1002%2Fpro.5560060501), [2](https://doi.org/10.1101%2Fcshperspect.a016295)]. Its levels increase with age [[3](https://doi.org/10.1186%2Fs12979-016-0076-x)] and may be associated with the risk of a wide range of diseases, including cardiovascular diseases [[4](https://doi.org/10.1186/s12916-022-02446-6)], autoimmune diseases [[5](https://doi.org/10.3389/fimmu.2023.1255533)], cancer [[6](https://doi.org/10.1093%2Fgerona%2F61.6.575)], type 2 diabetes [[7](https://doi.org/10.1001/jama.286.3.327)], rheumatoid arthritis [[8](https://doi.org/10.1002/art.1780310614)], and mortality risk, particularly from cardiovascular diseases [[9](https://doi.org/10.1016/S0002-9343(99)00066-2)].</t>
   </si>
   <si>
-    <t>#### CCL11</t>
-  </si>
-  <si>
-    <t>#### IL27</t>
-  </si>
-  <si>
-    <t>#### IL5</t>
-  </si>
-  <si>
-    <t>#### IL1B</t>
-  </si>
-  <si>
-    <t>#### GCSF</t>
-  </si>
-  <si>
-    <t>#### CXCL10</t>
-  </si>
-  <si>
-    <t>#### VEGFA</t>
-  </si>
-  <si>
-    <t>#### TNF</t>
-  </si>
-  <si>
-    <t>#### PDGFB</t>
-  </si>
-  <si>
-    <t>#### IL8</t>
-  </si>
-  <si>
-    <t>#### PDGFA</t>
-  </si>
-  <si>
-    <t>#### IL12Bp40</t>
-  </si>
-  <si>
-    <t>#### IL15</t>
-  </si>
-  <si>
-    <t>#### CXCL1</t>
-  </si>
-  <si>
-    <t>#### CCL4</t>
-  </si>
-  <si>
-    <t>#### IFNA2</t>
-  </si>
-  <si>
-    <t>#### IL13</t>
-  </si>
-  <si>
-    <t>#### FLT3L</t>
-  </si>
-  <si>
-    <t>#### CD40LG</t>
-  </si>
-  <si>
-    <t>#### CCL22</t>
-  </si>
-  <si>
-    <t>#### CSF-1
+    <t>#### IL15
+Interleukin-15 is a proinflammatory cytokine [[1](https://doi.org/10.1016/B978-0-12-814841-9.00050-6), [2](https://doi.org/10.1016/j.autrev.2006.08.015)] that plays an important role in the development of inflammatory and protective immune responses by modulating immune cells of the innate and adaptive immune system [[3](https://doi.org/10.1016/j.micinf.2011.10.006)]. Its production is associated with increased osteoclastogenesis and bone destruction in rheumatoid arthritis [[1](https://doi.org/10.1016/B978-0-12-814841-9.00050-6)], and it contributes to the development and progression of various hematologic malignancies [[4](https://doi.org/10.3389/fimmu.2023.1141208)]. Elevated levels of IL15 can be observed in obese patients and serve as a risk marker for atherosclerosis [[5](https://doi.org/10.3389/fmed.2021.634962)]. Disturbed IL15 expression has been reported in patients with a number of inflammatory autoimmune diseases, including rheumatoid arthritis, sarcoidosis, chronic hepatitis C, ulcerative colitis, and psoriasis [[6](https://doi.org/10.1186/ar1202), [7](https://doi.org/10.1016/j.cyto.2020.155258)].</t>
+  </si>
+  <si>
+    <t>#### CSF1
 Colony Stimulating Factor-1 is one of the best known proinflammatory cytokines responsible for a variety of inflammatory diseases [[1](https://doi.org/10.1016/j.biopha.2018.04.046)]. Its levels depend on age [[2](https://doi.org/10.1038/s41598-017-07698-4), [3](https://doi.org/10.3389/fimmu.2023.1177611)] and can be associated with bad habits, including smoking [[4](https://doi.org/10.1038/s41598-017-07698-4)], as well as with various diseases such as periodontitis [[4](https://doi.org/10.1038/s41598-017-07698-4)], chronic kidney disease [[5](https://doi.org/10.1007%2Fs11357-022-00540-4)], atherosclerosis and cancer [[6](https://doi.org/10.1016/j.coi.2005.11.006)].</t>
   </si>
 </sst>
@@ -350,7 +370,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -364,6 +384,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -648,38 +671,38 @@
   <dimension ref="A1:T25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="6" ySplit="27" topLeftCell="M31" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="27" topLeftCell="T28" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A28" sqref="A28"/>
-      <selection pane="bottomRight" activeCell="T12" sqref="T12"/>
+      <selection pane="bottomRight" activeCell="T39" sqref="T39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.36328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.81640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.81640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.36328125" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.36328125" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="28.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="25.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.81640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="23.6328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="23.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="20" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.81640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="20.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="6.90625" style="3" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="6.6328125" style="3" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="134.81640625" style="3" customWidth="1"/>
-    <col min="21" max="16384" width="8.7265625" style="3"/>
+    <col min="16" max="16" width="11.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="6.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="134.85546875" style="3" customWidth="1"/>
+    <col min="21" max="16384" width="8.7109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -741,7 +764,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>19</v>
       </c>
@@ -800,10 +823,10 @@
         <v>5</v>
       </c>
       <c r="T2" s="5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>22</v>
       </c>
@@ -861,11 +884,11 @@
       <c r="S3" s="3">
         <v>5</v>
       </c>
-      <c r="T3" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="T3" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>25</v>
       </c>
@@ -923,11 +946,11 @@
       <c r="S4" s="3">
         <v>5</v>
       </c>
-      <c r="T4" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="T4" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>27</v>
       </c>
@@ -985,11 +1008,11 @@
       <c r="S5" s="3">
         <v>5</v>
       </c>
-      <c r="T5" s="4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="T5" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>29</v>
       </c>
@@ -1051,7 +1074,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:20" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>31</v>
       </c>
@@ -1110,10 +1133,10 @@
         <v>5</v>
       </c>
       <c r="T7" s="5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>33</v>
       </c>
@@ -1171,11 +1194,11 @@
       <c r="S8" s="3">
         <v>5</v>
       </c>
-      <c r="T8" s="4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" ht="20.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="T8" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>35</v>
       </c>
@@ -1234,10 +1257,10 @@
         <v>5</v>
       </c>
       <c r="T9" s="5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>36</v>
       </c>
@@ -1295,11 +1318,11 @@
       <c r="S10" s="3">
         <v>5</v>
       </c>
-      <c r="T10" s="4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="T10" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>37</v>
       </c>
@@ -1357,11 +1380,11 @@
       <c r="S11" s="3">
         <v>5</v>
       </c>
-      <c r="T11" s="4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="T11" s="6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>39</v>
       </c>
@@ -1419,11 +1442,11 @@
       <c r="S12" s="3">
         <v>5</v>
       </c>
-      <c r="T12" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="T12" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>41</v>
       </c>
@@ -1481,11 +1504,11 @@
       <c r="S13" s="3">
         <v>5</v>
       </c>
-      <c r="T13" s="4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="T13" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>42</v>
       </c>
@@ -1543,11 +1566,11 @@
       <c r="S14" s="3">
         <v>5</v>
       </c>
-      <c r="T14" s="4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="T14" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>44</v>
       </c>
@@ -1605,11 +1628,11 @@
       <c r="S15" s="3">
         <v>5</v>
       </c>
-      <c r="T15" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="T15" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>45</v>
       </c>
@@ -1667,11 +1690,11 @@
       <c r="S16" s="3">
         <v>5</v>
       </c>
-      <c r="T16" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="T16" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>46</v>
       </c>
@@ -1729,11 +1752,11 @@
       <c r="S17" s="3">
         <v>5</v>
       </c>
-      <c r="T17" s="4" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="T17" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>47</v>
       </c>
@@ -1791,11 +1814,11 @@
       <c r="S18" s="3">
         <v>5</v>
       </c>
-      <c r="T18" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="T18" s="6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>49</v>
       </c>
@@ -1853,11 +1876,11 @@
       <c r="S19" s="3">
         <v>5</v>
       </c>
-      <c r="T19" s="4" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="T19" s="6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>51</v>
       </c>
@@ -1915,11 +1938,11 @@
       <c r="S20" s="3">
         <v>5</v>
       </c>
-      <c r="T20" s="4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="T20" s="6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>53</v>
       </c>
@@ -1977,11 +2000,11 @@
       <c r="S21" s="3">
         <v>5</v>
       </c>
-      <c r="T21" s="4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="T21" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>54</v>
       </c>
@@ -2039,11 +2062,11 @@
       <c r="S22" s="3">
         <v>5</v>
       </c>
-      <c r="T22" s="4" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="T22" s="6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>56</v>
       </c>
@@ -2101,11 +2124,11 @@
       <c r="S23" s="3">
         <v>5</v>
       </c>
-      <c r="T23" s="4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="T23" s="6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>58</v>
       </c>
@@ -2163,11 +2186,11 @@
       <c r="S24" s="3">
         <v>5</v>
       </c>
-      <c r="T24" s="4" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="T24" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>59</v>
       </c>
@@ -2225,8 +2248,8 @@
       <c r="S25" s="3">
         <v>5</v>
       </c>
-      <c r="T25" s="4" t="s">
-        <v>84</v>
+      <c r="T25" s="6" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>